<commit_message>
Corrected absolute path to xlsx file.
</commit_message>
<xml_diff>
--- a/10. ADO.NET-HW/ADO.NET/07. WritingToExcelFile/scores.xlsx
+++ b/10. ADO.NET-HW/ADO.NET/07. WritingToExcelFile/scores.xlsx
@@ -13,11 +13,6 @@
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -428,7 +423,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>

</xml_diff>